<commit_message>
reporte cierre de mes funcionando html
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/inventarios.xlsx
+++ b/public/application/files/jasper/templates/inventarios.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>CLAVE</t>
   </si>
@@ -172,7 +172,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -184,8 +184,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -202,45 +204,50 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -688,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:I5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -699,150 +706,176 @@
     <col min="1" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.75" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="29.75" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="29.75" customHeight="1">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="28">
-      <c r="A3" s="10" t="s">
+    <row r="4" spans="1:9" ht="28">
+      <c r="A4" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" ht="22.25" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>9</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="14"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+    <row r="5" spans="1:9" ht="22.25" customHeight="1">
+      <c r="A5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="G5" s="13"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="A6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="10">
-    <mergeCell ref="B7:D7"/>
+  <mergeCells count="11">
+    <mergeCell ref="B1:D1"/>
     <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A3:I3"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Requisicion y estadistico mensual
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/inventarios.xlsx
+++ b/public/application/files/jasper/templates/inventarios.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>CLAVE</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>{prod:subcat}</t>
+  </si>
+  <si>
+    <t>SUBCATEGORIA</t>
   </si>
 </sst>
 </file>
@@ -122,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -152,6 +158,24 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -159,20 +183,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -186,8 +208,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -222,32 +248,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,31 +729,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="6" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="10" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
@@ -727,11 +764,14 @@
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.75" customHeight="1">
+    <row r="2" spans="1:10" ht="29.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -743,8 +783,9 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="29.75" customHeight="1">
+    <row r="3" spans="1:10" ht="29.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -756,8 +797,9 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:9" ht="28">
+    <row r="4" spans="1:10" ht="28">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -769,8 +811,9 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="22.25" customHeight="1">
+    <row r="5" spans="1:10" ht="22.25" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
@@ -779,50 +822,53 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="8" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+    <row r="7" spans="1:10">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:10" s="1" customFormat="1">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>3</v>
@@ -830,28 +876,34 @@
       <c r="H8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -861,22 +913,24 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="11">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A7:J7"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>